<commit_message>
changed some things in the excel sheet
</commit_message>
<xml_diff>
--- a/Card Clash/Card Idea Things/Initial Card Ideas.xlsx
+++ b/Card Clash/Card Idea Things/Initial Card Ideas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Card Clash\Card Idea Things\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\CardClashPrototype\Card Clash\Card Idea Things\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E988BC9C-A5BA-4491-8857-97B07E21C101}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8597DDCE-A67E-4FD7-BDE8-8F97BF560395}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{2A6DB081-0EEE-462C-A19A-71EB81AAF283}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Card Name</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Haunty Squire</t>
+  </si>
+  <si>
+    <t>Protector</t>
+  </si>
+  <si>
+    <t>Armor</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533B3590-743A-4102-87F3-1A741B1717B2}">
-  <dimension ref="B3:G5"/>
+  <dimension ref="B3:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +425,7 @@
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -438,8 +444,11 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -453,7 +462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -470,6 +479,26 @@
         <v>25</v>
       </c>
       <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
         <v>10</v>
       </c>
     </row>

</xml_diff>